<commit_message>
Last commit after cleaning of the repository
</commit_message>
<xml_diff>
--- a/team9/files/Datasets/dataset_final_covid.xlsx
+++ b/team9/files/Datasets/dataset_final_covid.xlsx
@@ -459,19 +459,19 @@
         <v>37172386</v>
       </c>
       <c r="E3">
-        <v>8676</v>
+        <v>12456</v>
       </c>
       <c r="F3">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="G3">
-        <v>5.192026145429566</v>
+        <v>6.106683601101097</v>
       </c>
       <c r="H3">
-        <v>233.3990613354763</v>
+        <v>335.0874490542523</v>
       </c>
       <c r="I3">
-        <v>2.224527431996312</v>
+        <v>1.822414900449583</v>
       </c>
     </row>
     <row r="4">
@@ -494,19 +494,19 @@
         <v>30809762</v>
       </c>
       <c r="E4">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>0.09737173562067764</v>
+        <v>0.1298289808275702</v>
       </c>
       <c r="H4">
-        <v>1.882520221999768</v>
+        <v>2.304464409689371</v>
       </c>
       <c r="I4">
-        <v>5.172413793103448</v>
+        <v>5.633802816901409</v>
       </c>
     </row>
     <row r="5">
@@ -529,19 +529,19 @@
         <v>2866376</v>
       </c>
       <c r="E5">
-        <v>969</v>
+        <v>1050</v>
       </c>
       <c r="F5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G5">
-        <v>10.81505008414807</v>
+        <v>11.5127952508673</v>
       </c>
       <c r="H5">
-        <v>338.057533275467</v>
+        <v>366.3162125275958</v>
       </c>
       <c r="I5">
-        <v>3.199174406604747</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
     <row r="6">
@@ -564,7 +564,7 @@
         <v>77006</v>
       </c>
       <c r="E6">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="F6">
         <v>51</v>
@@ -573,10 +573,10 @@
         <v>662.2860556320287</v>
       </c>
       <c r="H6">
-        <v>9895.332831207957</v>
+        <v>9908.318832298781</v>
       </c>
       <c r="I6">
-        <v>6.692913385826772</v>
+        <v>6.684141546526867</v>
       </c>
     </row>
     <row r="7">
@@ -599,19 +599,19 @@
         <v>9630959</v>
       </c>
       <c r="E7">
-        <v>26898</v>
+        <v>31969</v>
       </c>
       <c r="F7">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="G7">
-        <v>24.60814130763094</v>
+        <v>26.47711406517253</v>
       </c>
       <c r="H7">
-        <v>2792.868290686317</v>
+        <v>3319.399449213729</v>
       </c>
       <c r="I7">
-        <v>0.8811064019629712</v>
+        <v>0.7976477212299415</v>
       </c>
     </row>
     <row r="8">
@@ -634,19 +634,19 @@
         <v>44494502</v>
       </c>
       <c r="E8">
-        <v>9918</v>
+        <v>13920</v>
       </c>
       <c r="F8">
-        <v>416</v>
+        <v>500</v>
       </c>
       <c r="G8">
-        <v>9.349469738980336</v>
+        <v>11.23734343627444</v>
       </c>
       <c r="H8">
-        <v>222.9039444019398</v>
+        <v>312.8476412658804</v>
       </c>
       <c r="I8">
-        <v>4.194394031054649</v>
+        <v>3.591954022988506</v>
       </c>
     </row>
     <row r="9">
@@ -669,19 +669,19 @@
         <v>2951776</v>
       </c>
       <c r="E9">
-        <v>5606</v>
+        <v>7774</v>
       </c>
       <c r="F9">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="G9">
-        <v>23.71453660440358</v>
+        <v>33.20035124616502</v>
       </c>
       <c r="H9">
-        <v>1899.195602918379</v>
+        <v>2633.668679466193</v>
       </c>
       <c r="I9">
-        <v>1.248662147698894</v>
+        <v>1.260612297401595</v>
       </c>
     </row>
     <row r="10">
@@ -739,19 +739,19 @@
         <v>24992369</v>
       </c>
       <c r="E11">
-        <v>7081</v>
+        <v>7139</v>
       </c>
       <c r="F11">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G11">
-        <v>4.001221332799624</v>
+        <v>4.121257972783613</v>
       </c>
       <c r="H11">
-        <v>283.3264825755414</v>
+        <v>285.6471909485651</v>
       </c>
       <c r="I11">
-        <v>1.412229911029516</v>
+        <v>1.442779100714386</v>
       </c>
     </row>
     <row r="12">
@@ -774,19 +774,19 @@
         <v>8847037</v>
       </c>
       <c r="E12">
-        <v>16332</v>
+        <v>16515</v>
       </c>
       <c r="F12">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="G12">
-        <v>71.54937862246987</v>
+        <v>72.90576494706646</v>
       </c>
       <c r="H12">
-        <v>1846.041787775953</v>
+        <v>1866.72667922605</v>
       </c>
       <c r="I12">
-        <v>3.87582659808964</v>
+        <v>3.905540417801998</v>
       </c>
     </row>
     <row r="13">
@@ -809,19 +809,19 @@
         <v>9942334</v>
       </c>
       <c r="E13">
-        <v>3749</v>
+        <v>4568</v>
       </c>
       <c r="F13">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G13">
-        <v>4.425520204813075</v>
+        <v>5.431320251361501</v>
       </c>
       <c r="H13">
-        <v>377.074437451005</v>
+        <v>459.449461263321</v>
       </c>
       <c r="I13">
-        <v>1.173646305681515</v>
+        <v>1.182136602451839</v>
       </c>
     </row>
     <row r="14">
@@ -879,19 +879,19 @@
         <v>11422068</v>
       </c>
       <c r="E15">
-        <v>56235</v>
+        <v>57592</v>
       </c>
       <c r="F15">
-        <v>9186</v>
+        <v>9364</v>
       </c>
       <c r="G15">
-        <v>804.2326485886794</v>
+        <v>819.8165165887648</v>
       </c>
       <c r="H15">
-        <v>4923.364140364074</v>
+        <v>5042.16924640967</v>
       </c>
       <c r="I15">
-        <v>16.33502267271273</v>
+        <v>16.25920266703709</v>
       </c>
     </row>
     <row r="16">
@@ -914,7 +914,7 @@
         <v>11485048</v>
       </c>
       <c r="E16">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -923,10 +923,10 @@
         <v>0.2612091825824324</v>
       </c>
       <c r="H16">
-        <v>11.75441321620946</v>
+        <v>18.28464278077027</v>
       </c>
       <c r="I16">
-        <v>2.222222222222222</v>
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="17">
@@ -949,19 +949,19 @@
         <v>19751535</v>
       </c>
       <c r="E17">
-        <v>812</v>
+        <v>845</v>
       </c>
       <c r="F17">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17">
-        <v>2.632706774435506</v>
+        <v>2.683335750866958</v>
       </c>
       <c r="H17">
-        <v>41.11072886233905</v>
+        <v>42.78148508457697</v>
       </c>
       <c r="I17">
-        <v>6.403940886699508</v>
+        <v>6.272189349112427</v>
       </c>
     </row>
     <row r="18">
@@ -984,19 +984,19 @@
         <v>161356039</v>
       </c>
       <c r="E18">
-        <v>28511</v>
+        <v>38292</v>
       </c>
       <c r="F18">
-        <v>408</v>
+        <v>544</v>
       </c>
       <c r="G18">
-        <v>2.528569754987602</v>
+        <v>3.371426339983469</v>
       </c>
       <c r="H18">
-        <v>176.6962065795381</v>
+        <v>237.3137084754541</v>
       </c>
       <c r="I18">
-        <v>1.431026621304058</v>
+        <v>1.420662279327275</v>
       </c>
     </row>
     <row r="19">
@@ -1019,19 +1019,19 @@
         <v>7024216</v>
       </c>
       <c r="E19">
-        <v>2372</v>
+        <v>2460</v>
       </c>
       <c r="F19">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G19">
-        <v>17.79558031814511</v>
+        <v>18.9344974585064</v>
       </c>
       <c r="H19">
-        <v>337.6889321171217</v>
+        <v>350.2170206610958</v>
       </c>
       <c r="I19">
-        <v>5.269814502529511</v>
+        <v>5.40650406504065</v>
       </c>
     </row>
     <row r="20">
@@ -1054,19 +1054,19 @@
         <v>1569439</v>
       </c>
       <c r="E20">
-        <v>8174</v>
+        <v>9633</v>
       </c>
       <c r="F20">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G20">
-        <v>7.646044223445448</v>
+        <v>9.557555279306811</v>
       </c>
       <c r="H20">
-        <v>5208.230456870258</v>
+        <v>6137.862000370834</v>
       </c>
       <c r="I20">
-        <v>0.1468069488622462</v>
+        <v>0.155714730613516</v>
       </c>
     </row>
     <row r="21">
@@ -1089,7 +1089,7 @@
         <v>385640</v>
       </c>
       <c r="E21">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F21">
         <v>11</v>
@@ -1098,10 +1098,10 @@
         <v>28.5240120319469</v>
       </c>
       <c r="H21">
-        <v>251.5299242817135</v>
+        <v>259.3092002904263</v>
       </c>
       <c r="I21">
-        <v>11.34020618556701</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22">
@@ -1124,19 +1124,19 @@
         <v>3323929</v>
       </c>
       <c r="E22">
-        <v>2352</v>
+        <v>2435</v>
       </c>
       <c r="F22">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="G22">
-        <v>41.81798106999277</v>
+        <v>45.42816648610726</v>
       </c>
       <c r="H22">
-        <v>707.5963415584389</v>
+        <v>732.566790686564</v>
       </c>
       <c r="I22">
-        <v>5.909863945578231</v>
+        <v>6.201232032854209</v>
       </c>
     </row>
     <row r="23">
@@ -1159,19 +1159,19 @@
         <v>9485386</v>
       </c>
       <c r="E23">
-        <v>33371</v>
+        <v>38956</v>
       </c>
       <c r="F23">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="G23">
-        <v>19.50368704025329</v>
+        <v>22.56102176548218</v>
       </c>
       <c r="H23">
-        <v>3518.148866055636</v>
+        <v>4106.949364000579</v>
       </c>
       <c r="I23">
-        <v>0.5543735578795961</v>
+        <v>0.5493377143443885</v>
       </c>
     </row>
     <row r="24">
@@ -1229,7 +1229,7 @@
         <v>63968</v>
       </c>
       <c r="E25">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="F25">
         <v>9</v>
@@ -1238,10 +1238,10 @@
         <v>140.6953476738369</v>
       </c>
       <c r="H25">
-        <v>1954.102051025513</v>
+        <v>2172.96148074037</v>
       </c>
       <c r="I25">
-        <v>7.199999999999999</v>
+        <v>6.474820143884892</v>
       </c>
     </row>
     <row r="26">
@@ -1264,19 +1264,19 @@
         <v>11353142</v>
       </c>
       <c r="E26">
-        <v>5187</v>
+        <v>7768</v>
       </c>
       <c r="F26">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="G26">
-        <v>18.93748884669989</v>
+        <v>24.66277617244636</v>
       </c>
       <c r="H26">
-        <v>456.8779285945688</v>
+        <v>684.2158760984404</v>
       </c>
       <c r="I26">
-        <v>4.144977829188355</v>
+        <v>3.604531410916581</v>
       </c>
     </row>
     <row r="27">
@@ -1299,19 +1299,19 @@
         <v>209469333</v>
       </c>
       <c r="E27">
-        <v>310087</v>
+        <v>411821</v>
       </c>
       <c r="F27">
-        <v>20047</v>
+        <v>25598</v>
       </c>
       <c r="G27">
-        <v>95.70374676277793</v>
+        <v>122.2040459736414</v>
       </c>
       <c r="H27">
-        <v>1480.345574022523</v>
+        <v>1966.020486636104</v>
       </c>
       <c r="I27">
-        <v>6.46495983385308</v>
+        <v>6.215807353194713</v>
       </c>
     </row>
     <row r="28">
@@ -1334,7 +1334,7 @@
         <v>286641</v>
       </c>
       <c r="E28">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F28">
         <v>7</v>
@@ -1343,10 +1343,10 @@
         <v>24.42079116386002</v>
       </c>
       <c r="H28">
-        <v>313.9816006782003</v>
+        <v>320.9589695821603</v>
       </c>
       <c r="I28">
-        <v>7.777777777777778</v>
+        <v>7.608695652173914</v>
       </c>
     </row>
     <row r="29">
@@ -1372,16 +1372,16 @@
         <v>141</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>2.331208825024128</v>
+        <v>4.662417650048257</v>
       </c>
       <c r="H29">
         <v>328.7004443284021</v>
       </c>
       <c r="I29">
-        <v>0.7092198581560284</v>
+        <v>1.418439716312057</v>
       </c>
     </row>
     <row r="30">
@@ -1404,7 +1404,7 @@
         <v>754394</v>
       </c>
       <c r="E30">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>27.83691280683568</v>
+        <v>37.11588374244758</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>2254126</v>
       </c>
       <c r="E31">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1448,10 +1448,10 @@
         <v>0.4436309239146348</v>
       </c>
       <c r="H31">
-        <v>12.86529679352441</v>
+        <v>15.52708233701222</v>
       </c>
       <c r="I31">
-        <v>3.448275862068965</v>
+        <v>2.857142857142857</v>
       </c>
     </row>
     <row r="32">
@@ -1474,19 +1474,19 @@
         <v>4666377</v>
       </c>
       <c r="E32">
-        <v>436</v>
+        <v>702</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>0.214299016131787</v>
       </c>
       <c r="H32">
-        <v>93.43437103345916</v>
+        <v>150.4379093245145</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>0.1424501424501425</v>
       </c>
     </row>
     <row r="33">
@@ -1509,19 +1509,19 @@
         <v>37058856</v>
       </c>
       <c r="E33">
-        <v>81313</v>
+        <v>87508</v>
       </c>
       <c r="F33">
-        <v>6152</v>
+        <v>6765</v>
       </c>
       <c r="G33">
-        <v>166.0062037532945</v>
+        <v>182.5474591012739</v>
       </c>
       <c r="H33">
-        <v>2194.158394959629</v>
+        <v>2361.324915156582</v>
       </c>
       <c r="I33">
-        <v>7.565825882700183</v>
+        <v>7.730721762581706</v>
       </c>
     </row>
     <row r="34">
@@ -1544,19 +1544,19 @@
         <v>8516543</v>
       </c>
       <c r="E34">
-        <v>30611</v>
+        <v>30678</v>
       </c>
       <c r="F34">
-        <v>1637</v>
+        <v>1647</v>
       </c>
       <c r="G34">
-        <v>192.2141413481973</v>
+        <v>193.3883266954679</v>
       </c>
       <c r="H34">
-        <v>3594.298766530034</v>
+        <v>3602.165808356748</v>
       </c>
       <c r="I34">
-        <v>5.347750808532881</v>
+        <v>5.368668100919225</v>
       </c>
     </row>
     <row r="35">
@@ -1579,19 +1579,19 @@
         <v>18729160</v>
       </c>
       <c r="E35">
-        <v>57581</v>
+        <v>82289</v>
       </c>
       <c r="F35">
-        <v>589</v>
+        <v>841</v>
       </c>
       <c r="G35">
-        <v>31.44828705611998</v>
+        <v>44.90324178980798</v>
       </c>
       <c r="H35">
-        <v>3074.403763970194</v>
+        <v>4393.630040001794</v>
       </c>
       <c r="I35">
-        <v>1.022906861638388</v>
+        <v>1.022007801771804</v>
       </c>
     </row>
     <row r="36">
@@ -1614,7 +1614,7 @@
         <v>1392730000</v>
       </c>
       <c r="E36">
-        <v>84079</v>
+        <v>84106</v>
       </c>
       <c r="F36">
         <v>4638</v>
@@ -1623,10 +1623,10 @@
         <v>3.330150136781716</v>
       </c>
       <c r="H36">
-        <v>60.36992094663</v>
+        <v>60.38930733164361</v>
       </c>
       <c r="I36">
-        <v>5.516240678409591</v>
+        <v>5.514469835683542</v>
       </c>
     </row>
     <row r="37">
@@ -1649,19 +1649,19 @@
         <v>25069229</v>
       </c>
       <c r="E37">
-        <v>2231</v>
+        <v>2556</v>
       </c>
       <c r="F37">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G37">
-        <v>1.156796645002525</v>
+        <v>1.236575723968216</v>
       </c>
       <c r="H37">
-        <v>88.99356258622872</v>
+        <v>101.9576629181536</v>
       </c>
       <c r="I37">
-        <v>1.29986553115195</v>
+        <v>1.21283255086072</v>
       </c>
     </row>
     <row r="38">
@@ -1684,19 +1684,19 @@
         <v>25216237</v>
       </c>
       <c r="E38">
-        <v>4288</v>
+        <v>5436</v>
       </c>
       <c r="F38">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="G38">
-        <v>6.186490077801854</v>
+        <v>7.019286819044412</v>
       </c>
       <c r="H38">
-        <v>170.0491631641946</v>
+        <v>215.5753850187877</v>
       </c>
       <c r="I38">
-        <v>3.638059701492538</v>
+        <v>3.2560706401766</v>
       </c>
     </row>
     <row r="39">
@@ -1719,19 +1719,19 @@
         <v>84068091</v>
       </c>
       <c r="E39">
-        <v>1945</v>
+        <v>2659</v>
       </c>
       <c r="F39">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G39">
-        <v>0.7493925370566581</v>
+        <v>0.8088681352357578</v>
       </c>
       <c r="H39">
-        <v>23.13600769166984</v>
+        <v>31.6291231116453</v>
       </c>
       <c r="I39">
-        <v>3.239074550128534</v>
+        <v>2.557352388115833</v>
       </c>
     </row>
     <row r="40">
@@ -1754,19 +1754,19 @@
         <v>5244363</v>
       </c>
       <c r="E40">
-        <v>469</v>
+        <v>571</v>
       </c>
       <c r="F40">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G40">
-        <v>3.050894836989735</v>
+        <v>3.622937618925311</v>
       </c>
       <c r="H40">
-        <v>89.42935490926162</v>
+        <v>108.8788094950712</v>
       </c>
       <c r="I40">
-        <v>3.411513859275053</v>
+        <v>3.327495621716287</v>
       </c>
     </row>
     <row r="41">
@@ -1789,19 +1789,19 @@
         <v>49648685</v>
       </c>
       <c r="E41">
-        <v>18330</v>
+        <v>24104</v>
       </c>
       <c r="F41">
-        <v>652</v>
+        <v>803</v>
       </c>
       <c r="G41">
-        <v>13.13227127767835</v>
+        <v>16.17364085272349</v>
       </c>
       <c r="H41">
-        <v>369.1940682819696</v>
+        <v>485.4912068668082</v>
       </c>
       <c r="I41">
-        <v>3.557010365521004</v>
+        <v>3.331397278460007</v>
       </c>
     </row>
     <row r="42">
@@ -1824,19 +1824,19 @@
         <v>832322</v>
       </c>
       <c r="E42">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>1.201458089537463</v>
+        <v>2.402916179074925</v>
       </c>
       <c r="H42">
-        <v>40.84957504427373</v>
+        <v>104.5268537897593</v>
       </c>
       <c r="I42">
-        <v>2.941176470588235</v>
+        <v>2.298850574712644</v>
       </c>
     </row>
     <row r="43">
@@ -1859,19 +1859,19 @@
         <v>543767</v>
       </c>
       <c r="E43">
-        <v>356</v>
+        <v>390</v>
       </c>
       <c r="F43">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G43">
-        <v>5.51706889163925</v>
+        <v>7.356091855519</v>
       </c>
       <c r="H43">
-        <v>654.692175141191</v>
+        <v>717.2189559131025</v>
       </c>
       <c r="I43">
-        <v>0.8426966292134831</v>
+        <v>1.025641025641026</v>
       </c>
     </row>
     <row r="44">
@@ -1894,7 +1894,7 @@
         <v>4999441</v>
       </c>
       <c r="E44">
-        <v>903</v>
+        <v>984</v>
       </c>
       <c r="F44">
         <v>10</v>
@@ -1903,10 +1903,10 @@
         <v>2.000223625001275</v>
       </c>
       <c r="H44">
-        <v>180.6201933376151</v>
+        <v>196.8220047001255</v>
       </c>
       <c r="I44">
-        <v>1.107419712070875</v>
+        <v>1.016260162601626</v>
       </c>
     </row>
     <row r="45">
@@ -1929,19 +1929,19 @@
         <v>11338138</v>
       </c>
       <c r="E45">
-        <v>1908</v>
+        <v>1974</v>
       </c>
       <c r="F45">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G45">
-        <v>7.055832271577573</v>
+        <v>7.232228078367013</v>
       </c>
       <c r="H45">
-        <v>168.2815996771251</v>
+        <v>174.1026613011766</v>
       </c>
       <c r="I45">
-        <v>4.19287211740042</v>
+        <v>4.154002026342452</v>
       </c>
     </row>
     <row r="46">
@@ -1964,7 +1964,7 @@
         <v>159849</v>
       </c>
       <c r="E46">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1973,10 +1973,10 @@
         <v>6.25590400940888</v>
       </c>
       <c r="H46">
-        <v>100.0944641505421</v>
+        <v>112.6062721693598</v>
       </c>
       <c r="I46">
-        <v>6.25</v>
+        <v>5.555555555555555</v>
       </c>
     </row>
     <row r="47">
@@ -1999,7 +1999,7 @@
         <v>64174</v>
       </c>
       <c r="E47">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2008,10 +2008,10 @@
         <v>15.58263471187709</v>
       </c>
       <c r="H47">
-        <v>1729.672453018356</v>
+        <v>2181.568859662792</v>
       </c>
       <c r="I47">
-        <v>0.9009009009009009</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="48">
@@ -2034,7 +2034,7 @@
         <v>1189265</v>
       </c>
       <c r="E48">
-        <v>923</v>
+        <v>939</v>
       </c>
       <c r="F48">
         <v>17</v>
@@ -2043,10 +2043,10 @@
         <v>14.29454326832119</v>
       </c>
       <c r="H48">
-        <v>776.1096139212035</v>
+        <v>789.5633017031528</v>
       </c>
       <c r="I48">
-        <v>1.841820151679306</v>
+        <v>1.810436634717785</v>
       </c>
     </row>
     <row r="49">
@@ -2069,19 +2069,19 @@
         <v>10625695</v>
       </c>
       <c r="E49">
-        <v>8754</v>
+        <v>9086</v>
       </c>
       <c r="F49">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="G49">
-        <v>28.79811626439494</v>
+        <v>29.8333426660562</v>
       </c>
       <c r="H49">
-        <v>823.8519927402397</v>
+        <v>855.0970077721975</v>
       </c>
       <c r="I49">
-        <v>3.495544893762851</v>
+        <v>3.488883997358574</v>
       </c>
     </row>
     <row r="50">
@@ -2104,19 +2104,19 @@
         <v>82927922</v>
       </c>
       <c r="E50">
-        <v>177212</v>
+        <v>179717</v>
       </c>
       <c r="F50">
-        <v>8174</v>
+        <v>8411</v>
       </c>
       <c r="G50">
-        <v>98.56752469934072</v>
+        <v>101.4254282170485</v>
       </c>
       <c r="H50">
-        <v>2136.940076709025</v>
+        <v>2167.147031611379</v>
       </c>
       <c r="I50">
-        <v>4.61255445455161</v>
+        <v>4.680135991586773</v>
       </c>
     </row>
     <row r="51">
@@ -2139,19 +2139,19 @@
         <v>958920</v>
       </c>
       <c r="E51">
-        <v>2047</v>
+        <v>2697</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G51">
-        <v>10.42839861510866</v>
+        <v>18.77111750719559</v>
       </c>
       <c r="H51">
-        <v>2134.693196512744</v>
+        <v>2812.539106494807</v>
       </c>
       <c r="I51">
-        <v>0.4885197850512946</v>
+        <v>0.6674082313681869</v>
       </c>
     </row>
     <row r="52">
@@ -2209,19 +2209,19 @@
         <v>5797446</v>
       </c>
       <c r="E53">
-        <v>11182</v>
+        <v>11480</v>
       </c>
       <c r="F53">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="G53">
-        <v>96.76674866829291</v>
+        <v>97.45670766058019</v>
       </c>
       <c r="H53">
-        <v>1928.780362939129</v>
+        <v>1980.182307864532</v>
       </c>
       <c r="I53">
-        <v>5.016991593632624</v>
+        <v>4.921602787456446</v>
       </c>
     </row>
     <row r="54">
@@ -2244,19 +2244,19 @@
         <v>10627165</v>
       </c>
       <c r="E54">
-        <v>13657</v>
+        <v>15723</v>
       </c>
       <c r="F54">
-        <v>448</v>
+        <v>474</v>
       </c>
       <c r="G54">
-        <v>42.15611595378448</v>
+        <v>44.60267625467375</v>
       </c>
       <c r="H54">
-        <v>1285.102847278649</v>
+        <v>1479.510292726235</v>
       </c>
       <c r="I54">
-        <v>3.28036904151717</v>
+        <v>3.014691852699867</v>
       </c>
     </row>
     <row r="55">
@@ -2279,19 +2279,19 @@
         <v>42228429</v>
       </c>
       <c r="E55">
-        <v>7728</v>
+        <v>8857</v>
       </c>
       <c r="F55">
-        <v>575</v>
+        <v>623</v>
       </c>
       <c r="G55">
-        <v>13.61641940314663</v>
+        <v>14.75309441419192</v>
       </c>
       <c r="H55">
-        <v>183.0046767782908</v>
+        <v>209.7402202672517</v>
       </c>
       <c r="I55">
-        <v>7.440476190476191</v>
+        <v>7.033984419103534</v>
       </c>
     </row>
     <row r="56">
@@ -2314,19 +2314,19 @@
         <v>17084357</v>
       </c>
       <c r="E56">
-        <v>35306</v>
+        <v>38103</v>
       </c>
       <c r="F56">
-        <v>2939</v>
+        <v>3275</v>
       </c>
       <c r="G56">
-        <v>172.0287160939098</v>
+        <v>191.6958302849794</v>
       </c>
       <c r="H56">
-        <v>2066.568850089003</v>
+        <v>2230.285869114067</v>
       </c>
       <c r="I56">
-        <v>8.32436413074265</v>
+        <v>8.595123743537254</v>
       </c>
     </row>
     <row r="57">
@@ -2349,19 +2349,19 @@
         <v>98423595</v>
       </c>
       <c r="E57">
-        <v>15003</v>
+        <v>19666</v>
       </c>
       <c r="F57">
-        <v>696</v>
+        <v>816</v>
       </c>
       <c r="G57">
-        <v>7.071475086842743</v>
+        <v>8.290694929401836</v>
       </c>
       <c r="H57">
-        <v>152.4329608159507</v>
+        <v>199.8098118647262</v>
       </c>
       <c r="I57">
-        <v>4.639072185562887</v>
+        <v>4.149293196379538</v>
       </c>
     </row>
     <row r="58">
@@ -2410,19 +2410,19 @@
         <v>46723749</v>
       </c>
       <c r="E59">
-        <v>233037</v>
+        <v>236769</v>
       </c>
       <c r="F59">
-        <v>27940</v>
+        <v>27118</v>
       </c>
       <c r="G59">
-        <v>597.9828373789098</v>
+        <v>580.3900710107829</v>
       </c>
       <c r="H59">
-        <v>4987.549265363959</v>
+        <v>5067.422992962316</v>
       </c>
       <c r="I59">
-        <v>11.9895123950274</v>
+        <v>11.45335749190139</v>
       </c>
     </row>
     <row r="60">
@@ -2445,19 +2445,19 @@
         <v>1320884</v>
       </c>
       <c r="E60">
-        <v>1800</v>
+        <v>1840</v>
       </c>
       <c r="F60">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G60">
-        <v>48.45240005935419</v>
+        <v>49.96653756120901</v>
       </c>
       <c r="H60">
-        <v>1362.723751669336</v>
+        <v>1393.006501706433</v>
       </c>
       <c r="I60">
-        <v>3.555555555555555</v>
+        <v>3.58695652173913</v>
       </c>
     </row>
     <row r="61">
@@ -2480,19 +2480,19 @@
         <v>109224559</v>
       </c>
       <c r="E61">
-        <v>399</v>
+        <v>731</v>
       </c>
       <c r="F61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G61">
-        <v>0.04577725051744086</v>
+        <v>0.05493270062092903</v>
       </c>
       <c r="H61">
-        <v>3.653024591291781</v>
+        <v>6.692634025649854</v>
       </c>
       <c r="I61">
-        <v>1.2531328320802</v>
+        <v>0.8207934336525308</v>
       </c>
     </row>
     <row r="62">
@@ -2515,19 +2515,19 @@
         <v>5518050</v>
       </c>
       <c r="E62">
-        <v>6493</v>
+        <v>6692</v>
       </c>
       <c r="F62">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G62">
-        <v>55.45437246853508</v>
+        <v>56.72293654461268</v>
       </c>
       <c r="H62">
-        <v>1176.683792281694</v>
+        <v>1212.747256730185</v>
       </c>
       <c r="I62">
-        <v>4.712767595872478</v>
+        <v>4.677226539151225</v>
       </c>
     </row>
     <row r="63">
@@ -2585,19 +2585,19 @@
         <v>66987244</v>
       </c>
       <c r="E64">
-        <v>144163</v>
+        <v>145746</v>
       </c>
       <c r="F64">
-        <v>28215</v>
+        <v>28596</v>
       </c>
       <c r="G64">
-        <v>421.1995943585916</v>
+        <v>426.8872443834232</v>
       </c>
       <c r="H64">
-        <v>2152.096300603142</v>
+        <v>2175.727665404476</v>
       </c>
       <c r="I64">
-        <v>19.57159604059294</v>
+        <v>19.62043555226215</v>
       </c>
     </row>
     <row r="65">
@@ -2655,19 +2655,19 @@
         <v>2119275</v>
       </c>
       <c r="E66">
-        <v>1567</v>
+        <v>2319</v>
       </c>
       <c r="F66">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G66">
-        <v>5.662313762961389</v>
+        <v>6.606032723454955</v>
       </c>
       <c r="H66">
-        <v>739.4038055467081</v>
+        <v>1094.242134692289</v>
       </c>
       <c r="I66">
-        <v>0.7657945118059988</v>
+        <v>0.603708495040966</v>
       </c>
     </row>
     <row r="67">
@@ -2690,19 +2690,19 @@
         <v>66488991</v>
       </c>
       <c r="E67">
-        <v>250908</v>
+        <v>267240</v>
       </c>
       <c r="F67">
-        <v>36042</v>
+        <v>37460</v>
       </c>
       <c r="G67">
-        <v>542.0747022616119</v>
+        <v>563.4015411664166</v>
       </c>
       <c r="H67">
-        <v>3773.677359609804</v>
+        <v>4019.312009111403</v>
       </c>
       <c r="I67">
-        <v>14.36462767229423</v>
+        <v>14.01736267025894</v>
       </c>
     </row>
     <row r="68">
@@ -2725,7 +2725,7 @@
         <v>3731000</v>
       </c>
       <c r="E68">
-        <v>721</v>
+        <v>735</v>
       </c>
       <c r="F68">
         <v>12</v>
@@ -2734,10 +2734,10 @@
         <v>3.216295899222729</v>
       </c>
       <c r="H68">
-        <v>193.2457786116323</v>
+        <v>196.9981238273921</v>
       </c>
       <c r="I68">
-        <v>1.664355062413315</v>
+        <v>1.63265306122449</v>
       </c>
     </row>
     <row r="69">
@@ -2760,19 +2760,19 @@
         <v>29767108</v>
       </c>
       <c r="E69">
-        <v>6486</v>
+        <v>7303</v>
       </c>
       <c r="F69">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G69">
-        <v>1.041417930152973</v>
+        <v>1.142200310490358</v>
       </c>
       <c r="H69">
-        <v>217.8915062894253</v>
+        <v>245.3379078679729</v>
       </c>
       <c r="I69">
-        <v>0.4779525131051496</v>
+        <v>0.4655620977680405</v>
       </c>
     </row>
     <row r="70">
@@ -2795,7 +2795,7 @@
         <v>33718</v>
       </c>
       <c r="E70">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -2804,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>4478.320185064357</v>
+        <v>4656.266682484134</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -2830,19 +2830,19 @@
         <v>12414318</v>
       </c>
       <c r="E71">
-        <v>3067</v>
+        <v>3446</v>
       </c>
       <c r="F71">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G71">
-        <v>1.530490841301149</v>
+        <v>1.691595140385481</v>
       </c>
       <c r="H71">
-        <v>247.0534426458223</v>
+        <v>277.5827073223032</v>
       </c>
       <c r="I71">
-        <v>0.6194978806651451</v>
+        <v>0.6094022054556006</v>
       </c>
     </row>
     <row r="72">
@@ -2865,7 +2865,7 @@
         <v>2280102</v>
       </c>
       <c r="E72">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2874,10 +2874,10 @@
         <v>0.4385768706838554</v>
       </c>
       <c r="H72">
-        <v>10.52584489641253</v>
+        <v>10.96442176709638</v>
       </c>
       <c r="I72">
-        <v>4.166666666666666</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
@@ -2900,19 +2900,19 @@
         <v>1874309</v>
       </c>
       <c r="E73">
-        <v>1089</v>
+        <v>1178</v>
       </c>
       <c r="F73">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G73">
-        <v>3.201179741440712</v>
+        <v>3.734709698347498</v>
       </c>
       <c r="H73">
-        <v>581.0141230714893</v>
+        <v>628.4982892361932</v>
       </c>
       <c r="I73">
-        <v>0.5509641873278237</v>
+        <v>0.5942275042444821</v>
       </c>
     </row>
     <row r="74">
@@ -2935,19 +2935,19 @@
         <v>1308974</v>
       </c>
       <c r="E74">
-        <v>903</v>
+        <v>1043</v>
       </c>
       <c r="F74">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G74">
-        <v>7.639571145034202</v>
+        <v>9.167485374041043</v>
       </c>
       <c r="H74">
-        <v>689.8532743965885</v>
+        <v>796.8072704270674</v>
       </c>
       <c r="I74">
-        <v>1.107419712070875</v>
+        <v>1.150527325023969</v>
       </c>
     </row>
     <row r="75">
@@ -2970,19 +2970,19 @@
         <v>10727668</v>
       </c>
       <c r="E75">
-        <v>2853</v>
+        <v>2903</v>
       </c>
       <c r="F75">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="G75">
-        <v>15.66043990175684</v>
+        <v>16.12652442264246</v>
       </c>
       <c r="H75">
-        <v>265.9478276173349</v>
+        <v>270.6086728261911</v>
       </c>
       <c r="I75">
-        <v>5.888538380651945</v>
+        <v>5.959352394075094</v>
       </c>
     </row>
     <row r="76">
@@ -3005,7 +3005,7 @@
         <v>111454</v>
       </c>
       <c r="E76">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
       <c r="H76">
-        <v>197.3908518312488</v>
+        <v>206.3631632781237</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -3040,7 +3040,7 @@
         <v>56025</v>
       </c>
       <c r="E77">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>196.3409192324855</v>
+        <v>214.190093708166</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -3075,19 +3075,19 @@
         <v>17247807</v>
       </c>
       <c r="E78">
-        <v>2512</v>
+        <v>4145</v>
       </c>
       <c r="F78">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G78">
-        <v>2.782962494884132</v>
+        <v>3.942530201085854</v>
       </c>
       <c r="H78">
-        <v>145.6417038989362</v>
+        <v>240.3204071103068</v>
       </c>
       <c r="I78">
-        <v>1.910828025477707</v>
+        <v>1.640530759951749</v>
       </c>
     </row>
     <row r="79">
@@ -3110,7 +3110,7 @@
         <v>165768</v>
       </c>
       <c r="E79">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F79">
         <v>5</v>
@@ -3119,10 +3119,10 @@
         <v>30.1626369383717</v>
       </c>
       <c r="H79">
-        <v>995.3670189662661</v>
+        <v>1031.562183292312</v>
       </c>
       <c r="I79">
-        <v>3.03030303030303</v>
+        <v>2.923976608187134</v>
       </c>
     </row>
     <row r="80">
@@ -3145,19 +3145,19 @@
         <v>779004</v>
       </c>
       <c r="E80">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F80">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G80">
-        <v>12.83690456018198</v>
+        <v>14.12059501620017</v>
       </c>
       <c r="H80">
-        <v>163.0286879143111</v>
+        <v>178.4329733865295</v>
       </c>
       <c r="I80">
-        <v>7.874015748031496</v>
+        <v>7.913669064748201</v>
       </c>
     </row>
     <row r="81">
@@ -3180,19 +3180,19 @@
         <v>9587522</v>
       </c>
       <c r="E81">
-        <v>3204</v>
+        <v>4640</v>
       </c>
       <c r="F81">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="G81">
-        <v>16.27114910401249</v>
+        <v>20.23463414216938</v>
       </c>
       <c r="H81">
-        <v>334.1843700593334</v>
+        <v>483.9623836065252</v>
       </c>
       <c r="I81">
-        <v>4.868913857677903</v>
+        <v>4.181034482758621</v>
       </c>
     </row>
     <row r="82">
@@ -3215,19 +3215,19 @@
         <v>4089400</v>
       </c>
       <c r="E82">
-        <v>2237</v>
+        <v>2244</v>
       </c>
       <c r="F82">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G82">
-        <v>23.71986110431848</v>
+        <v>24.69799970655842</v>
       </c>
       <c r="H82">
-        <v>547.024013302685</v>
+        <v>548.7357558566049</v>
       </c>
       <c r="I82">
-        <v>4.336164506034868</v>
+        <v>4.500891265597148</v>
       </c>
     </row>
     <row r="83">
@@ -3250,19 +3250,19 @@
         <v>11123176</v>
       </c>
       <c r="E83">
-        <v>734</v>
+        <v>1320</v>
       </c>
       <c r="F83">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G83">
-        <v>2.247559509981681</v>
+        <v>3.056680933575087</v>
       </c>
       <c r="H83">
-        <v>65.98834721306217</v>
+        <v>118.6711421270328</v>
       </c>
       <c r="I83">
-        <v>3.40599455040872</v>
+        <v>2.575757575757576</v>
       </c>
     </row>
     <row r="84">
@@ -3285,19 +3285,19 @@
         <v>9768785</v>
       </c>
       <c r="E84">
-        <v>3678</v>
+        <v>3816</v>
       </c>
       <c r="F84">
-        <v>476</v>
+        <v>509</v>
       </c>
       <c r="G84">
-        <v>48.7266328412387</v>
+        <v>52.10473973989601</v>
       </c>
       <c r="H84">
-        <v>376.5053688867142</v>
+        <v>390.6319977356447</v>
       </c>
       <c r="I84">
-        <v>12.94181620445895</v>
+        <v>13.33857442348008</v>
       </c>
     </row>
     <row r="85">
@@ -3320,19 +3320,19 @@
         <v>267663435</v>
       </c>
       <c r="E85">
-        <v>20162</v>
+        <v>23851</v>
       </c>
       <c r="F85">
-        <v>1278</v>
+        <v>1473</v>
       </c>
       <c r="G85">
-        <v>4.774652914396021</v>
+        <v>5.503179767531564</v>
       </c>
       <c r="H85">
-        <v>75.32594057907087</v>
+        <v>89.10817422633764</v>
       </c>
       <c r="I85">
-        <v>6.33865687927785</v>
+        <v>6.175841683786843</v>
       </c>
     </row>
     <row r="86">
@@ -3355,19 +3355,19 @@
         <v>1352617328</v>
       </c>
       <c r="E86">
-        <v>118447</v>
+        <v>158333</v>
       </c>
       <c r="F86">
-        <v>3583</v>
+        <v>4531</v>
       </c>
       <c r="G86">
-        <v>2.648938414309594</v>
+        <v>3.349801829538591</v>
       </c>
       <c r="H86">
-        <v>87.56874361142296</v>
+        <v>117.056758569043</v>
       </c>
       <c r="I86">
-        <v>3.024981637356793</v>
+        <v>2.861690235137337</v>
       </c>
     </row>
     <row r="87">
@@ -3390,19 +3390,19 @@
         <v>4853506</v>
       </c>
       <c r="E87">
-        <v>24391</v>
+        <v>24803</v>
       </c>
       <c r="F87">
-        <v>1583</v>
+        <v>1631</v>
       </c>
       <c r="G87">
-        <v>326.1559787914139</v>
+        <v>336.0457368343626</v>
       </c>
       <c r="H87">
-        <v>5025.439342199227</v>
+        <v>5110.32643206787</v>
       </c>
       <c r="I87">
-        <v>6.490098806936985</v>
+        <v>6.575817441438536</v>
       </c>
     </row>
     <row r="88">
@@ -3425,19 +3425,19 @@
         <v>81800269</v>
       </c>
       <c r="E88">
-        <v>129341</v>
+        <v>141591</v>
       </c>
       <c r="F88">
-        <v>7249</v>
+        <v>7564</v>
       </c>
       <c r="G88">
-        <v>88.61829048508386</v>
+        <v>92.4691335672747</v>
       </c>
       <c r="H88">
-        <v>1581.180619344907</v>
+        <v>1730.935628096773</v>
       </c>
       <c r="I88">
-        <v>5.604564677867033</v>
+        <v>5.34214745287483</v>
       </c>
     </row>
     <row r="89">
@@ -3460,19 +3460,19 @@
         <v>38433600</v>
       </c>
       <c r="E89">
-        <v>3877</v>
+        <v>5135</v>
       </c>
       <c r="F89">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="G89">
-        <v>3.642646018067524</v>
+        <v>4.553307522584405</v>
       </c>
       <c r="H89">
-        <v>100.8752758003414</v>
+        <v>133.607052162691</v>
       </c>
       <c r="I89">
-        <v>3.611039463502709</v>
+        <v>3.407984420642649</v>
       </c>
     </row>
     <row r="90">
@@ -3495,7 +3495,7 @@
         <v>353574</v>
       </c>
       <c r="E90">
-        <v>1803</v>
+        <v>1805</v>
       </c>
       <c r="F90">
         <v>10</v>
@@ -3504,10 +3504,10 @@
         <v>28.28262259102762</v>
       </c>
       <c r="H90">
-        <v>5099.35685316228</v>
+        <v>5105.013377680485</v>
       </c>
       <c r="I90">
-        <v>0.5546311702717693</v>
+        <v>0.554016620498615</v>
       </c>
     </row>
     <row r="91">
@@ -3530,19 +3530,19 @@
         <v>8883800</v>
       </c>
       <c r="E91">
-        <v>16690</v>
+        <v>16793</v>
       </c>
       <c r="F91">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G91">
-        <v>31.40547963709224</v>
+        <v>31.63060852337964</v>
       </c>
       <c r="H91">
-        <v>1878.700556068349</v>
+        <v>1890.29469371215</v>
       </c>
       <c r="I91">
-        <v>1.671659676452966</v>
+        <v>1.673316262728518</v>
       </c>
     </row>
     <row r="92">
@@ -3565,19 +3565,19 @@
         <v>60431283</v>
       </c>
       <c r="E92">
-        <v>228006</v>
+        <v>231139</v>
       </c>
       <c r="F92">
-        <v>32486</v>
+        <v>33072</v>
       </c>
       <c r="G92">
-        <v>537.569258623882</v>
+        <v>547.266223025581</v>
       </c>
       <c r="H92">
-        <v>3772.979633743669</v>
+        <v>3824.823643079033</v>
       </c>
       <c r="I92">
-        <v>14.24787067007009</v>
+        <v>14.30827337662618</v>
       </c>
     </row>
     <row r="93">
@@ -3600,7 +3600,7 @@
         <v>2934855</v>
       </c>
       <c r="E93">
-        <v>534</v>
+        <v>569</v>
       </c>
       <c r="F93">
         <v>9</v>
@@ -3609,10 +3609,10 @@
         <v>3.066591024088072</v>
       </c>
       <c r="H93">
-        <v>181.9510674292256</v>
+        <v>193.8766991895681</v>
       </c>
       <c r="I93">
-        <v>1.685393258426966</v>
+        <v>1.581722319859403</v>
       </c>
     </row>
     <row r="94">
@@ -3635,7 +3635,7 @@
         <v>9956011</v>
       </c>
       <c r="E94">
-        <v>684</v>
+        <v>720</v>
       </c>
       <c r="F94">
         <v>9</v>
@@ -3644,10 +3644,10 @@
         <v>0.9039765022356845</v>
       </c>
       <c r="H94">
-        <v>68.70221416991203</v>
+        <v>72.31812017885477</v>
       </c>
       <c r="I94">
-        <v>1.31578947368421</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="95">
@@ -3670,19 +3670,19 @@
         <v>126529100</v>
       </c>
       <c r="E95">
-        <v>16513</v>
+        <v>16651</v>
       </c>
       <c r="F95">
-        <v>796</v>
+        <v>858</v>
       </c>
       <c r="G95">
-        <v>6.291042930045342</v>
+        <v>6.781048786405656</v>
       </c>
       <c r="H95">
-        <v>130.5075275173853</v>
+        <v>131.5981857138002</v>
       </c>
       <c r="I95">
-        <v>4.820444498274087</v>
+        <v>5.152843673052669</v>
       </c>
     </row>
     <row r="96">
@@ -3705,19 +3705,19 @@
         <v>18276499</v>
       </c>
       <c r="E96">
-        <v>7597</v>
+        <v>9576</v>
       </c>
       <c r="F96">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G96">
-        <v>1.915027599104183</v>
+        <v>2.024457747624422</v>
       </c>
       <c r="H96">
-        <v>415.670419154128</v>
+        <v>523.9515511149044</v>
       </c>
       <c r="I96">
-        <v>0.4607081742793208</v>
+        <v>0.3863826232247285</v>
       </c>
     </row>
     <row r="97">
@@ -3740,19 +3740,19 @@
         <v>51393010</v>
       </c>
       <c r="E97">
-        <v>1109</v>
+        <v>1471</v>
       </c>
       <c r="F97">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G97">
-        <v>0.9728949520567096</v>
+        <v>1.070184447262381</v>
       </c>
       <c r="H97">
-        <v>21.57881003661782</v>
+        <v>28.6225694895084</v>
       </c>
       <c r="I97">
-        <v>4.508566275924256</v>
+        <v>3.738953093133922</v>
       </c>
     </row>
     <row r="98">
@@ -3775,19 +3775,19 @@
         <v>6315800</v>
       </c>
       <c r="E98">
-        <v>1350</v>
+        <v>1594</v>
       </c>
       <c r="F98">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G98">
-        <v>2.21666297222838</v>
+        <v>2.533329111118148</v>
       </c>
       <c r="H98">
-        <v>213.7496437505937</v>
+        <v>252.3829126951455</v>
       </c>
       <c r="I98">
-        <v>1.037037037037037</v>
+        <v>1.003764115432873</v>
       </c>
     </row>
     <row r="99">
@@ -3810,7 +3810,7 @@
         <v>16249798</v>
       </c>
       <c r="E99">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3819,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>7.569324861761359</v>
+        <v>7.630864088279744</v>
       </c>
       <c r="I99">
         <v>0</v>
@@ -3880,19 +3880,19 @@
         <v>51635256</v>
       </c>
       <c r="E101">
-        <v>11142</v>
+        <v>11344</v>
       </c>
       <c r="F101">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G101">
-        <v>5.112785729192473</v>
+        <v>5.209618792245361</v>
       </c>
       <c r="H101">
-        <v>215.782797707055</v>
+        <v>219.6948534543917</v>
       </c>
       <c r="I101">
-        <v>2.369413031771674</v>
+        <v>2.3712976022567</v>
       </c>
     </row>
     <row r="102">
@@ -3915,19 +3915,19 @@
         <v>4137309</v>
       </c>
       <c r="E102">
-        <v>18609</v>
+        <v>23267</v>
       </c>
       <c r="F102">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="G102">
-        <v>31.17968708646127</v>
+        <v>42.29802511729243</v>
       </c>
       <c r="H102">
-        <v>4497.851139472541</v>
+        <v>5623.70371659453</v>
       </c>
       <c r="I102">
-        <v>0.6932129614702564</v>
+        <v>0.7521382215154511</v>
       </c>
     </row>
     <row r="103">
@@ -3985,7 +3985,7 @@
         <v>6848925</v>
       </c>
       <c r="E104">
-        <v>1024</v>
+        <v>1161</v>
       </c>
       <c r="F104">
         <v>26</v>
@@ -3994,10 +3994,10 @@
         <v>3.796216194512277</v>
       </c>
       <c r="H104">
-        <v>149.5125147377143</v>
+        <v>169.5156539164905</v>
       </c>
       <c r="I104">
-        <v>2.5390625</v>
+        <v>2.239448751076658</v>
       </c>
     </row>
     <row r="105">
@@ -4020,19 +4020,19 @@
         <v>4818977</v>
       </c>
       <c r="E105">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="F105">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G105">
-        <v>4.772797214014509</v>
+        <v>5.602848903408337</v>
       </c>
       <c r="H105">
-        <v>49.80310136362966</v>
+        <v>55.19843734468954</v>
       </c>
       <c r="I105">
-        <v>9.583333333333334</v>
+        <v>10.15037593984962</v>
       </c>
     </row>
     <row r="106">
@@ -4055,19 +4055,19 @@
         <v>6678567</v>
       </c>
       <c r="E106">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="F106">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G106">
-        <v>0.4491981588265866</v>
+        <v>0.5989308784354488</v>
       </c>
       <c r="H106">
-        <v>10.63102309222922</v>
+        <v>14.82353924127736</v>
       </c>
       <c r="I106">
-        <v>4.225352112676056</v>
+        <v>4.040404040404041</v>
       </c>
     </row>
     <row r="107">
@@ -4125,19 +4125,19 @@
         <v>21670000</v>
       </c>
       <c r="E108">
-        <v>1055</v>
+        <v>1469</v>
       </c>
       <c r="F108">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G108">
-        <v>0.4153207198892478</v>
+        <v>0.4614674665436087</v>
       </c>
       <c r="H108">
-        <v>48.68481772035071</v>
+        <v>67.78957083525611</v>
       </c>
       <c r="I108">
-        <v>0.8530805687203791</v>
+        <v>0.6807351940095302</v>
       </c>
     </row>
     <row r="109">
@@ -4160,7 +4160,7 @@
         <v>2108132</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -4169,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="H109">
-        <v>0.4743535983515264</v>
+        <v>0.9487071967030528</v>
       </c>
       <c r="I109">
         <v>0</v>
@@ -4195,19 +4195,19 @@
         <v>2789533</v>
       </c>
       <c r="E110">
-        <v>1594</v>
+        <v>1647</v>
       </c>
       <c r="F110">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G110">
-        <v>21.86745953534158</v>
+        <v>23.65987425135318</v>
       </c>
       <c r="H110">
-        <v>571.4218114644996</v>
+        <v>590.4214074542226</v>
       </c>
       <c r="I110">
-        <v>3.82685069008783</v>
+        <v>4.007285974499089</v>
       </c>
     </row>
     <row r="111">
@@ -4230,19 +4230,19 @@
         <v>607728</v>
       </c>
       <c r="E111">
-        <v>3980</v>
+        <v>4001</v>
       </c>
       <c r="F111">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G111">
-        <v>179.3565542479531</v>
+        <v>181.0020272227049</v>
       </c>
       <c r="H111">
-        <v>6548.982439512413</v>
+        <v>6583.537371982203</v>
       </c>
       <c r="I111">
-        <v>2.738693467336683</v>
+        <v>2.749312671832042</v>
       </c>
     </row>
     <row r="112">
@@ -4265,19 +4265,19 @@
         <v>1926542</v>
       </c>
       <c r="E112">
-        <v>1025</v>
+        <v>1057</v>
       </c>
       <c r="F112">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G112">
-        <v>11.41942402501477</v>
+        <v>11.93848875342453</v>
       </c>
       <c r="H112">
-        <v>532.0413466200062</v>
+        <v>548.6514179291186</v>
       </c>
       <c r="I112">
-        <v>2.146341463414634</v>
+        <v>2.1759697256386</v>
       </c>
     </row>
     <row r="113">
@@ -4300,19 +4300,19 @@
         <v>36029138</v>
       </c>
       <c r="E113">
-        <v>7211</v>
+        <v>7601</v>
       </c>
       <c r="F113">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G113">
-        <v>5.44004133543245</v>
+        <v>5.606573213047729</v>
       </c>
       <c r="H113">
-        <v>200.1435615806296</v>
+        <v>210.9681336256227</v>
       </c>
       <c r="I113">
-        <v>2.718069615864651</v>
+        <v>2.657545059860545</v>
       </c>
     </row>
     <row r="114">
@@ -4335,19 +4335,19 @@
         <v>3545883</v>
       </c>
       <c r="E114">
-        <v>6704</v>
+        <v>7537</v>
       </c>
       <c r="F114">
-        <v>233</v>
+        <v>274</v>
       </c>
       <c r="G114">
-        <v>65.71000791622285</v>
+        <v>77.2727131718672</v>
       </c>
       <c r="H114">
-        <v>1890.643317898532</v>
+        <v>2125.563646629063</v>
       </c>
       <c r="I114">
-        <v>3.475536992840095</v>
+        <v>3.635398699747911</v>
       </c>
     </row>
     <row r="115">
@@ -4370,7 +4370,7 @@
         <v>26262368</v>
       </c>
       <c r="E115">
-        <v>405</v>
+        <v>612</v>
       </c>
       <c r="F115">
         <v>2</v>
@@ -4379,10 +4379,10 @@
         <v>0.07615459504641775</v>
       </c>
       <c r="H115">
-        <v>15.42130549689959</v>
+        <v>23.30330608420383</v>
       </c>
       <c r="I115">
-        <v>0.4938271604938271</v>
+        <v>0.326797385620915</v>
       </c>
     </row>
     <row r="116">
@@ -4405,19 +4405,19 @@
         <v>515696</v>
       </c>
       <c r="E116">
-        <v>1216</v>
+        <v>1457</v>
       </c>
       <c r="F116">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G116">
-        <v>7.756507709968664</v>
+        <v>9.695634637460831</v>
       </c>
       <c r="H116">
-        <v>2357.978343830474</v>
+        <v>2825.307933356085</v>
       </c>
       <c r="I116">
-        <v>0.3289473684210526</v>
+        <v>0.3431708991077557</v>
       </c>
     </row>
     <row r="117">
@@ -4440,19 +4440,19 @@
         <v>126190788</v>
       </c>
       <c r="E117">
-        <v>59567</v>
+        <v>78023</v>
       </c>
       <c r="F117">
-        <v>6510</v>
+        <v>8597</v>
       </c>
       <c r="G117">
-        <v>51.5885517728917</v>
+        <v>68.12700147335636</v>
       </c>
       <c r="H117">
-        <v>472.0392109763194</v>
+        <v>618.2939439287755</v>
       </c>
       <c r="I117">
-        <v>10.92887001191935</v>
+        <v>11.01854581341399</v>
       </c>
     </row>
     <row r="118">
@@ -4475,19 +4475,19 @@
         <v>2082958</v>
       </c>
       <c r="E118">
-        <v>1898</v>
+        <v>2040</v>
       </c>
       <c r="F118">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G118">
-        <v>53.28960065445391</v>
+        <v>57.13029259351365</v>
       </c>
       <c r="H118">
-        <v>911.2041625419236</v>
+        <v>979.3764444602339</v>
       </c>
       <c r="I118">
-        <v>5.848261327713383</v>
+        <v>5.833333333333333</v>
       </c>
     </row>
     <row r="119">
@@ -4510,19 +4510,19 @@
         <v>19077690</v>
       </c>
       <c r="E119">
-        <v>947</v>
+        <v>1116</v>
       </c>
       <c r="F119">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G119">
-        <v>3.145034854848779</v>
+        <v>3.669207330656909</v>
       </c>
       <c r="H119">
-        <v>49.63913345902989</v>
+        <v>58.49764830018729</v>
       </c>
       <c r="I119">
-        <v>6.335797254487856</v>
+        <v>6.272401433691756</v>
       </c>
     </row>
     <row r="120">
@@ -4545,19 +4545,19 @@
         <v>483530</v>
       </c>
       <c r="E120">
-        <v>599</v>
+        <v>615</v>
       </c>
       <c r="F120">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G120">
-        <v>12.40874402829194</v>
+        <v>14.47686803300726</v>
       </c>
       <c r="H120">
-        <v>1238.806278824478</v>
+        <v>1271.896262899923</v>
       </c>
       <c r="I120">
-        <v>1.001669449081803</v>
+        <v>1.138211382113821</v>
       </c>
     </row>
     <row r="121">
@@ -4580,7 +4580,7 @@
         <v>53708395</v>
       </c>
       <c r="E121">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="F121">
         <v>6</v>
@@ -4589,10 +4589,10 @@
         <v>0.1117143791021869</v>
       </c>
       <c r="H121">
-        <v>3.705193573555866</v>
+        <v>3.83552701584175</v>
       </c>
       <c r="I121">
-        <v>3.015075376884422</v>
+        <v>2.912621359223301</v>
       </c>
     </row>
     <row r="122">
@@ -4650,7 +4650,7 @@
         <v>3170208</v>
       </c>
       <c r="E123">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -4659,7 +4659,7 @@
         <v>0</v>
       </c>
       <c r="H123">
-        <v>44.47657693122975</v>
+        <v>50.78531124771624</v>
       </c>
       <c r="I123">
         <v>0</v>
@@ -4720,19 +4720,19 @@
         <v>29495962</v>
       </c>
       <c r="E125">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>0.03390294576593229</v>
       </c>
       <c r="H125">
-        <v>5.492277214081033</v>
+        <v>7.695968688866632</v>
       </c>
       <c r="I125">
-        <v>0</v>
+        <v>0.4405286343612335</v>
       </c>
     </row>
     <row r="126">
@@ -4755,19 +4755,19 @@
         <v>4403319</v>
       </c>
       <c r="E126">
-        <v>173</v>
+        <v>292</v>
       </c>
       <c r="F126">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G126">
-        <v>1.135507102710478</v>
+        <v>3.63362272867353</v>
       </c>
       <c r="H126">
-        <v>39.28854575378254</v>
+        <v>66.31361479829192</v>
       </c>
       <c r="I126">
-        <v>2.890173410404624</v>
+        <v>5.47945205479452</v>
       </c>
     </row>
     <row r="127">
@@ -4825,7 +4825,7 @@
         <v>1265303</v>
       </c>
       <c r="E128">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F128">
         <v>10</v>
@@ -4834,10 +4834,10 @@
         <v>7.90324530962149</v>
       </c>
       <c r="H128">
-        <v>262.3877442794335</v>
+        <v>263.9683933413577</v>
       </c>
       <c r="I128">
-        <v>3.012048192771084</v>
+        <v>2.994011976047904</v>
       </c>
     </row>
     <row r="129">
@@ -4860,19 +4860,19 @@
         <v>18143315</v>
       </c>
       <c r="E129">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="F129">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G129">
-        <v>0.1653501578956216</v>
+        <v>0.2204668771941621</v>
       </c>
       <c r="H129">
-        <v>3.968403789494919</v>
+        <v>5.566788649152595</v>
       </c>
       <c r="I129">
-        <v>4.166666666666666</v>
+        <v>3.96039603960396</v>
       </c>
     </row>
     <row r="130">
@@ -4895,19 +4895,19 @@
         <v>31528585</v>
       </c>
       <c r="E130">
-        <v>7059</v>
+        <v>7619</v>
       </c>
       <c r="F130">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G130">
-        <v>3.61576645447298</v>
+        <v>3.647483704073621</v>
       </c>
       <c r="H130">
-        <v>223.892064930919</v>
+        <v>241.6537247072775</v>
       </c>
       <c r="I130">
-        <v>1.61495962600935</v>
+        <v>1.50938443365271</v>
       </c>
     </row>
     <row r="131">
@@ -4930,7 +4930,7 @@
         <v>2448255</v>
       </c>
       <c r="E131">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -4939,7 +4939,7 @@
         <v>0</v>
       </c>
       <c r="H131">
-        <v>7.352175324874247</v>
+        <v>8.985992063735191</v>
       </c>
       <c r="I131">
         <v>0</v>
@@ -5000,19 +5000,19 @@
         <v>22442948</v>
       </c>
       <c r="E133">
-        <v>924</v>
+        <v>955</v>
       </c>
       <c r="F133">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G133">
-        <v>2.673445574084118</v>
+        <v>2.851675279023059</v>
       </c>
       <c r="H133">
-        <v>41.17106184089541</v>
+        <v>42.55234205417221</v>
       </c>
       <c r="I133">
-        <v>6.493506493506493</v>
+        <v>6.701570680628273</v>
       </c>
     </row>
     <row r="134">
@@ -5035,19 +5035,19 @@
         <v>195874740</v>
       </c>
       <c r="E134">
-        <v>7016</v>
+        <v>8733</v>
       </c>
       <c r="F134">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="G134">
-        <v>1.077219043149719</v>
+        <v>1.296747094597292</v>
       </c>
       <c r="H134">
-        <v>35.81880951060867</v>
+        <v>44.58461565794548</v>
       </c>
       <c r="I134">
-        <v>3.007411630558723</v>
+        <v>2.90850795831902</v>
       </c>
     </row>
     <row r="135">
@@ -5070,19 +5070,19 @@
         <v>6465513</v>
       </c>
       <c r="E135">
-        <v>25</v>
+        <v>759</v>
       </c>
       <c r="F135">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="G135">
-        <v>1.237334145024533</v>
+        <v>5.413336884482329</v>
       </c>
       <c r="H135">
-        <v>3.866669203201664</v>
+        <v>117.3920770092025</v>
       </c>
       <c r="I135">
-        <v>32</v>
+        <v>4.61133069828722</v>
       </c>
     </row>
     <row r="136">
@@ -5105,19 +5105,19 @@
         <v>17231017</v>
       </c>
       <c r="E136">
-        <v>44700</v>
+        <v>45768</v>
       </c>
       <c r="F136">
-        <v>5775</v>
+        <v>5871</v>
       </c>
       <c r="G136">
-        <v>335.1514307019719</v>
+        <v>340.7227791603943</v>
       </c>
       <c r="H136">
-        <v>2594.159125952925</v>
+        <v>2656.140377552874</v>
       </c>
       <c r="I136">
-        <v>12.91946308724832</v>
+        <v>12.82773990561091</v>
       </c>
     </row>
     <row r="137">
@@ -5140,19 +5140,19 @@
         <v>5314336</v>
       </c>
       <c r="E137">
-        <v>8268</v>
+        <v>8383</v>
       </c>
       <c r="F137">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G137">
-        <v>44.03184141913496</v>
+        <v>44.2200116816099</v>
       </c>
       <c r="H137">
-        <v>1555.791730142769</v>
+        <v>1577.431310327386</v>
       </c>
       <c r="I137">
-        <v>2.830188679245283</v>
+        <v>2.803292377430514</v>
       </c>
     </row>
     <row r="138">
@@ -5175,19 +5175,19 @@
         <v>28087871</v>
       </c>
       <c r="E138">
-        <v>487</v>
+        <v>886</v>
       </c>
       <c r="F138">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G138">
-        <v>0.1068076679788226</v>
+        <v>0.1424102239717635</v>
       </c>
       <c r="H138">
-        <v>17.3384447685622</v>
+        <v>31.54386460974561</v>
       </c>
       <c r="I138">
-        <v>0.6160164271047228</v>
+        <v>0.4514672686230248</v>
       </c>
     </row>
     <row r="139">
@@ -5213,16 +5213,16 @@
         <v>1154</v>
       </c>
       <c r="F139">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G139">
-        <v>4.298434141848326</v>
+        <v>4.503121481936342</v>
       </c>
       <c r="H139">
         <v>236.20919046157</v>
       </c>
       <c r="I139">
-        <v>1.819757365684575</v>
+        <v>1.906412478336222</v>
       </c>
     </row>
     <row r="140">
@@ -5245,19 +5245,19 @@
         <v>4829483</v>
       </c>
       <c r="E140">
-        <v>6370</v>
+        <v>8373</v>
       </c>
       <c r="F140">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G140">
-        <v>6.418906537200773</v>
+        <v>7.868337045600947</v>
       </c>
       <c r="H140">
-        <v>1318.981762644159</v>
+        <v>1733.725949547809</v>
       </c>
       <c r="I140">
-        <v>0.4866562009419153</v>
+        <v>0.453839722918906</v>
       </c>
     </row>
     <row r="141">
@@ -5280,19 +5280,19 @@
         <v>212215030</v>
       </c>
       <c r="E141">
-        <v>50694</v>
+        <v>61227</v>
       </c>
       <c r="F141">
-        <v>1067</v>
+        <v>1260</v>
       </c>
       <c r="G141">
-        <v>5.027919087540595</v>
+        <v>5.937373992784583</v>
       </c>
       <c r="H141">
-        <v>238.8803469763664</v>
+        <v>288.5139662350966</v>
       </c>
       <c r="I141">
-        <v>2.104785576202312</v>
+        <v>2.057915625459356</v>
       </c>
     </row>
     <row r="142">
@@ -5315,19 +5315,19 @@
         <v>4176873</v>
       </c>
       <c r="E142">
-        <v>10116</v>
+        <v>11728</v>
       </c>
       <c r="F142">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="G142">
-        <v>69.6693435495884</v>
+        <v>75.41526879079159</v>
       </c>
       <c r="H142">
-        <v>2421.907489167135</v>
+        <v>2807.842134534615</v>
       </c>
       <c r="I142">
-        <v>2.876631079478055</v>
+        <v>2.685879945429741</v>
       </c>
     </row>
     <row r="143">
@@ -5350,19 +5350,19 @@
         <v>31989256</v>
       </c>
       <c r="E143">
-        <v>108769</v>
+        <v>135905</v>
       </c>
       <c r="F143">
-        <v>3148</v>
+        <v>3983</v>
       </c>
       <c r="G143">
-        <v>98.40804049959775</v>
+        <v>124.5105544186461</v>
       </c>
       <c r="H143">
-        <v>3400.172858037086</v>
+        <v>4248.457669662589</v>
       </c>
       <c r="I143">
-        <v>2.894206989123739</v>
+        <v>2.930723667267577</v>
       </c>
     </row>
     <row r="144">
@@ -5385,19 +5385,19 @@
         <v>106651922</v>
       </c>
       <c r="E144">
-        <v>13434</v>
+        <v>15049</v>
       </c>
       <c r="F144">
-        <v>846</v>
+        <v>904</v>
       </c>
       <c r="G144">
-        <v>7.932346498171875</v>
+        <v>8.476171671805409</v>
       </c>
       <c r="H144">
-        <v>125.9611617688428</v>
+        <v>141.1038799657075</v>
       </c>
       <c r="I144">
-        <v>6.297454220634211</v>
+        <v>6.007043657385873</v>
       </c>
     </row>
     <row r="145">
@@ -5455,19 +5455,19 @@
         <v>37978548</v>
       </c>
       <c r="E146">
-        <v>20143</v>
+        <v>22473</v>
       </c>
       <c r="F146">
-        <v>972</v>
+        <v>1028</v>
       </c>
       <c r="G146">
-        <v>25.59339551369894</v>
+        <v>27.06791212765691</v>
       </c>
       <c r="H146">
-        <v>530.3783599099154</v>
+        <v>591.7287833120951</v>
       </c>
       <c r="I146">
-        <v>4.825497691505734</v>
+        <v>4.57437814266008</v>
       </c>
     </row>
     <row r="147">
@@ -5490,19 +5490,19 @@
         <v>10281762</v>
       </c>
       <c r="E147">
-        <v>29912</v>
+        <v>31292</v>
       </c>
       <c r="F147">
-        <v>1277</v>
+        <v>1356</v>
       </c>
       <c r="G147">
-        <v>124.2005018206023</v>
+        <v>131.8840097640852</v>
       </c>
       <c r="H147">
-        <v>2909.228982347578</v>
+        <v>3043.447222372974</v>
       </c>
       <c r="I147">
-        <v>4.269189622893822</v>
+        <v>4.333375942732967</v>
       </c>
     </row>
     <row r="148">
@@ -5525,7 +5525,7 @@
         <v>6956071</v>
       </c>
       <c r="E148">
-        <v>836</v>
+        <v>884</v>
       </c>
       <c r="F148">
         <v>11</v>
@@ -5534,10 +5534,10 @@
         <v>1.581352461756069</v>
       </c>
       <c r="H148">
-        <v>120.1827870934612</v>
+        <v>127.0832341993059</v>
       </c>
       <c r="I148">
-        <v>1.31578947368421</v>
+        <v>1.244343891402715</v>
       </c>
     </row>
     <row r="149">
@@ -5560,19 +5560,19 @@
         <v>4569087</v>
       </c>
       <c r="E149">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="F149">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G149">
-        <v>0.8754484210959432</v>
+        <v>1.094310526369929</v>
       </c>
       <c r="H149">
-        <v>131.7549873749394</v>
+        <v>134.1624705329533</v>
       </c>
       <c r="I149">
-        <v>0.6644518272425249</v>
+        <v>0.8156606851549755</v>
       </c>
     </row>
     <row r="150">
@@ -5630,19 +5630,19 @@
         <v>2781677</v>
       </c>
       <c r="E151">
-        <v>38651</v>
+        <v>48947</v>
       </c>
       <c r="F151">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="G151">
-        <v>6.111421275726837</v>
+        <v>10.78486107481207</v>
       </c>
       <c r="H151">
-        <v>13894.8555134187</v>
+        <v>17596.2198342942</v>
       </c>
       <c r="I151">
-        <v>0.0439833380766345</v>
+        <v>0.06129078390912619</v>
       </c>
     </row>
     <row r="152">
@@ -5665,19 +5665,19 @@
         <v>19473936</v>
       </c>
       <c r="E152">
-        <v>17585</v>
+        <v>18594</v>
       </c>
       <c r="F152">
-        <v>1151</v>
+        <v>1219</v>
       </c>
       <c r="G152">
-        <v>59.10464119836894</v>
+        <v>62.59648794162619</v>
       </c>
       <c r="H152">
-        <v>903.0018379438035</v>
+        <v>954.8146815312529</v>
       </c>
       <c r="I152">
-        <v>6.545351151549617</v>
+        <v>6.555878240292568</v>
       </c>
     </row>
     <row r="153">
@@ -5700,19 +5700,19 @@
         <v>144478050</v>
       </c>
       <c r="E153">
-        <v>317554</v>
+        <v>370680</v>
       </c>
       <c r="F153">
-        <v>3099</v>
+        <v>3968</v>
       </c>
       <c r="G153">
-        <v>21.44962504684968</v>
+        <v>27.46437953723767</v>
       </c>
       <c r="H153">
-        <v>2197.939410173379</v>
+        <v>2565.649245681264</v>
       </c>
       <c r="I153">
-        <v>0.9758970127915252</v>
+        <v>1.07046509118377</v>
       </c>
     </row>
     <row r="154">
@@ -5735,7 +5735,7 @@
         <v>12301939</v>
       </c>
       <c r="E154">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="F154">
         <v>0</v>
@@ -5744,7 +5744,7 @@
         <v>0</v>
       </c>
       <c r="H154">
-        <v>26.01215954655603</v>
+        <v>28.12564750971371</v>
       </c>
       <c r="I154">
         <v>0</v>
@@ -5770,19 +5770,19 @@
         <v>33699947</v>
       </c>
       <c r="E155">
-        <v>65077</v>
+        <v>78541</v>
       </c>
       <c r="F155">
-        <v>351</v>
+        <v>425</v>
       </c>
       <c r="G155">
-        <v>10.41544664743835</v>
+        <v>12.61129579818034</v>
       </c>
       <c r="H155">
-        <v>1931.071286254545</v>
+        <v>2330.597137140898</v>
       </c>
       <c r="I155">
-        <v>0.5393610645850301</v>
+        <v>0.5411186514049987</v>
       </c>
     </row>
     <row r="156">
@@ -5805,19 +5805,19 @@
         <v>41801533</v>
       </c>
       <c r="E156">
-        <v>3138</v>
+        <v>4146</v>
       </c>
       <c r="F156">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="G156">
-        <v>2.894630682563723</v>
+        <v>4.401752442906819</v>
       </c>
       <c r="H156">
-        <v>75.06901720566086</v>
+        <v>99.18296537115039</v>
       </c>
       <c r="I156">
-        <v>3.855959209687699</v>
+        <v>4.438012542209358</v>
       </c>
     </row>
     <row r="157">
@@ -5840,19 +5840,19 @@
         <v>15854360</v>
       </c>
       <c r="E157">
-        <v>2812</v>
+        <v>3253</v>
       </c>
       <c r="F157">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G157">
-        <v>2.081446365542349</v>
+        <v>2.459891159277322</v>
       </c>
       <c r="H157">
-        <v>177.3644599971238</v>
+        <v>205.1801523366443</v>
       </c>
       <c r="I157">
-        <v>1.173541963015647</v>
+        <v>1.198893329234553</v>
       </c>
     </row>
     <row r="158">
@@ -5875,7 +5875,7 @@
         <v>5638676</v>
       </c>
       <c r="E158">
-        <v>29812</v>
+        <v>32876</v>
       </c>
       <c r="F158">
         <v>23</v>
@@ -5884,10 +5884,10 @@
         <v>4.078971730243057</v>
       </c>
       <c r="H158">
-        <v>5287.05674878287</v>
+        <v>5830.446721890033</v>
       </c>
       <c r="I158">
-        <v>0.07715014088286595</v>
+        <v>0.06995984913006449</v>
       </c>
     </row>
     <row r="159">
@@ -5910,19 +5910,19 @@
         <v>7650154</v>
       </c>
       <c r="E159">
-        <v>585</v>
+        <v>782</v>
       </c>
       <c r="F159">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G159">
-        <v>4.57507129921829</v>
+        <v>5.882234527566373</v>
       </c>
       <c r="H159">
-        <v>76.46904885836285</v>
+        <v>102.2201644568201</v>
       </c>
       <c r="I159">
-        <v>5.982905982905983</v>
+        <v>5.754475703324808</v>
       </c>
     </row>
     <row r="160">
@@ -5945,19 +5945,19 @@
         <v>6420744</v>
       </c>
       <c r="E160">
-        <v>1640</v>
+        <v>2109</v>
       </c>
       <c r="F160">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G160">
-        <v>5.139591299699848</v>
+        <v>6.074062445099821</v>
       </c>
       <c r="H160">
-        <v>255.4221130759925</v>
+        <v>328.4666076080903</v>
       </c>
       <c r="I160">
-        <v>2.01219512195122</v>
+        <v>1.849217638691323</v>
       </c>
     </row>
     <row r="161">
@@ -5980,19 +5980,19 @@
         <v>33785</v>
       </c>
       <c r="E161">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="F161">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G161">
-        <v>1213.556311972769</v>
+        <v>1243.155246411129</v>
       </c>
       <c r="H161">
-        <v>19476.09886044102</v>
+        <v>19742.48927038627</v>
       </c>
       <c r="I161">
-        <v>6.231003039513678</v>
+        <v>6.296851574212893</v>
       </c>
     </row>
     <row r="162">
@@ -6015,19 +6015,19 @@
         <v>15008154</v>
       </c>
       <c r="E162">
-        <v>1594</v>
+        <v>1731</v>
       </c>
       <c r="F162">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G162">
-        <v>4.064457227717679</v>
+        <v>4.464239905853844</v>
       </c>
       <c r="H162">
-        <v>106.2089314915079</v>
+        <v>115.3373026422837</v>
       </c>
       <c r="I162">
-        <v>3.82685069008783</v>
+        <v>3.870595031773541</v>
       </c>
     </row>
     <row r="163">
@@ -6050,19 +6050,19 @@
         <v>6982084</v>
       </c>
       <c r="E163">
-        <v>10919</v>
+        <v>11275</v>
       </c>
       <c r="F163">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G163">
-        <v>33.94402015214942</v>
+        <v>34.37369129331586</v>
       </c>
       <c r="H163">
-        <v>1563.85973013215</v>
+        <v>1614.847372217235</v>
       </c>
       <c r="I163">
-        <v>2.170528436670025</v>
+        <v>2.12860310421286</v>
       </c>
     </row>
     <row r="164">
@@ -6085,19 +6085,19 @@
         <v>10975920</v>
       </c>
       <c r="E164">
-        <v>339</v>
+        <v>806</v>
       </c>
       <c r="F164">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G164">
-        <v>0.546651214658999</v>
+        <v>0.7288682862119986</v>
       </c>
       <c r="H164">
-        <v>30.88579362823344</v>
+        <v>73.43347983585886</v>
       </c>
       <c r="I164">
-        <v>1.769911504424779</v>
+        <v>0.9925558312655087</v>
       </c>
     </row>
     <row r="165">
@@ -6120,19 +6120,19 @@
         <v>211028</v>
       </c>
       <c r="E165">
-        <v>251</v>
+        <v>443</v>
       </c>
       <c r="F165">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G165">
-        <v>37.90966127717649</v>
+        <v>56.86449191576473</v>
       </c>
       <c r="H165">
-        <v>1189.415622571412</v>
+        <v>2099.247493223648</v>
       </c>
       <c r="I165">
-        <v>3.187250996015936</v>
+        <v>2.708803611738149</v>
       </c>
     </row>
     <row r="166">
@@ -6155,7 +6155,7 @@
         <v>575991</v>
       </c>
       <c r="E166">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -6164,10 +6164,10 @@
         <v>1.736138238271084</v>
       </c>
       <c r="H166">
-        <v>19.09752062098193</v>
+        <v>20.83365885925301</v>
       </c>
       <c r="I166">
-        <v>9.090909090909092</v>
+        <v>8.333333333333332</v>
       </c>
     </row>
     <row r="167">
@@ -6190,7 +6190,7 @@
         <v>5447011</v>
       </c>
       <c r="E167">
-        <v>1502</v>
+        <v>1515</v>
       </c>
       <c r="F167">
         <v>28</v>
@@ -6199,10 +6199,10 @@
         <v>5.14043390035379</v>
       </c>
       <c r="H167">
-        <v>275.7475613689783</v>
+        <v>278.1341913941426</v>
       </c>
       <c r="I167">
-        <v>1.864181091877497</v>
+        <v>1.848184818481848</v>
       </c>
     </row>
     <row r="168">
@@ -6225,19 +6225,19 @@
         <v>2067372</v>
       </c>
       <c r="E168">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="F168">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G168">
-        <v>51.27282366211789</v>
+        <v>51.75652954572278</v>
       </c>
       <c r="H168">
-        <v>710.0802371319724</v>
+        <v>711.531354782787</v>
       </c>
       <c r="I168">
-        <v>7.220708446866484</v>
+        <v>7.273963290278722</v>
       </c>
     </row>
     <row r="169">
@@ -6260,19 +6260,19 @@
         <v>10183175</v>
       </c>
       <c r="E169">
-        <v>32172</v>
+        <v>35088</v>
       </c>
       <c r="F169">
-        <v>3871</v>
+        <v>4220</v>
       </c>
       <c r="G169">
-        <v>380.1368433715418</v>
+        <v>414.4090620066924</v>
       </c>
       <c r="H169">
-        <v>3159.328991203628</v>
+        <v>3445.683689026262</v>
       </c>
       <c r="I169">
-        <v>12.03220191470844</v>
+        <v>12.02690378476972</v>
       </c>
     </row>
     <row r="170">
@@ -6295,7 +6295,7 @@
         <v>1367000</v>
       </c>
       <c r="E170">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="F170">
         <v>2</v>
@@ -6304,10 +6304,10 @@
         <v>1.463057790782736</v>
       </c>
       <c r="H170">
-        <v>160.9363569861009</v>
+        <v>198.9758595464521</v>
       </c>
       <c r="I170">
-        <v>0.9090909090909091</v>
+        <v>0.7352941176470588</v>
       </c>
     </row>
     <row r="171">
@@ -6400,19 +6400,19 @@
         <v>16906283</v>
       </c>
       <c r="E173">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="F173">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G173">
-        <v>0.1774488218374198</v>
+        <v>0.2365984291165598</v>
       </c>
       <c r="H173">
-        <v>3.430677222190117</v>
+        <v>7.157102480775934</v>
       </c>
       <c r="I173">
-        <v>5.172413793103448</v>
+        <v>3.305785123966942</v>
       </c>
     </row>
     <row r="174">
@@ -6470,19 +6470,19 @@
         <v>15477751</v>
       </c>
       <c r="E175">
-        <v>588</v>
+        <v>715</v>
       </c>
       <c r="F175">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G175">
-        <v>3.747314451563409</v>
+        <v>4.134967670690658</v>
       </c>
       <c r="H175">
-        <v>37.99001547447042</v>
+        <v>46.19534194599719</v>
       </c>
       <c r="I175">
-        <v>9.863945578231291</v>
+        <v>8.951048951048952</v>
       </c>
     </row>
     <row r="176">
@@ -6505,19 +6505,19 @@
         <v>7889094</v>
       </c>
       <c r="E176">
-        <v>354</v>
+        <v>395</v>
       </c>
       <c r="F176">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G176">
-        <v>1.521087212295861</v>
+        <v>1.647844479987182</v>
       </c>
       <c r="H176">
-        <v>44.87207276272789</v>
+        <v>50.06912073807208</v>
       </c>
       <c r="I176">
-        <v>3.389830508474576</v>
+        <v>3.291139240506329</v>
       </c>
     </row>
     <row r="177">
@@ -6540,19 +6540,19 @@
         <v>69428524</v>
       </c>
       <c r="E177">
-        <v>3037</v>
+        <v>3054</v>
       </c>
       <c r="F177">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G177">
-        <v>0.8065849131403111</v>
+        <v>0.8209882151606738</v>
       </c>
       <c r="H177">
-        <v>43.74282823584151</v>
+        <v>43.98768437018767</v>
       </c>
       <c r="I177">
-        <v>1.843924925913731</v>
+        <v>1.866404715127701</v>
       </c>
     </row>
     <row r="178">
@@ -6575,19 +6575,19 @@
         <v>9100837</v>
       </c>
       <c r="E178">
-        <v>2140</v>
+        <v>3100</v>
       </c>
       <c r="F178">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G178">
-        <v>4.834720147168881</v>
+        <v>5.054480153858376</v>
       </c>
       <c r="H178">
-        <v>235.1432071577592</v>
+        <v>340.6280103687166</v>
       </c>
       <c r="I178">
-        <v>2.05607476635514</v>
+        <v>1.483870967741935</v>
       </c>
     </row>
     <row r="179">
@@ -6680,19 +6680,19 @@
         <v>11565204</v>
       </c>
       <c r="E181">
-        <v>1046</v>
+        <v>1051</v>
       </c>
       <c r="F181">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G181">
-        <v>4.063914480021277</v>
+        <v>4.150380745553646</v>
       </c>
       <c r="H181">
-        <v>90.44371374685652</v>
+        <v>90.87604507451836</v>
       </c>
       <c r="I181">
-        <v>4.493307839388145</v>
+        <v>4.567078972407232</v>
       </c>
     </row>
     <row r="182">
@@ -6715,19 +6715,19 @@
         <v>82319724</v>
       </c>
       <c r="E182">
-        <v>153548</v>
+        <v>158762</v>
       </c>
       <c r="F182">
-        <v>4249</v>
+        <v>4397</v>
       </c>
       <c r="G182">
-        <v>51.61581931445737</v>
+        <v>53.41368734423843</v>
       </c>
       <c r="H182">
-        <v>1865.263785383926</v>
+        <v>1928.602190162834</v>
       </c>
       <c r="I182">
-        <v>2.767212858519811</v>
+        <v>2.769554427381867</v>
       </c>
     </row>
     <row r="183">
@@ -6785,7 +6785,7 @@
         <v>42723139</v>
       </c>
       <c r="E184">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="F184">
         <v>0</v>
@@ -6794,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="H184">
-        <v>6.179321233863457</v>
+        <v>6.577232070892544</v>
       </c>
       <c r="I184">
         <v>0</v>
@@ -6820,19 +6820,19 @@
         <v>44622516</v>
       </c>
       <c r="E185">
-        <v>19706</v>
+        <v>21584</v>
       </c>
       <c r="F185">
-        <v>579</v>
+        <v>644</v>
       </c>
       <c r="G185">
-        <v>12.97551218313194</v>
+        <v>14.43217589971843</v>
       </c>
       <c r="H185">
-        <v>441.6156184469742</v>
+        <v>483.7019947508115</v>
       </c>
       <c r="I185">
-        <v>2.938191413782604</v>
+        <v>2.983691623424759</v>
       </c>
     </row>
     <row r="186">
@@ -6855,19 +6855,19 @@
         <v>3449299</v>
       </c>
       <c r="E186">
-        <v>749</v>
+        <v>803</v>
       </c>
       <c r="F186">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G186">
-        <v>5.79827959246212</v>
+        <v>6.378107551708333</v>
       </c>
       <c r="H186">
-        <v>217.1455707377064</v>
+        <v>232.8009256373541</v>
       </c>
       <c r="I186">
-        <v>2.67022696929239</v>
+        <v>2.73972602739726</v>
       </c>
     </row>
     <row r="187">
@@ -6890,19 +6890,19 @@
         <v>327167434</v>
       </c>
       <c r="E187">
-        <v>1577287</v>
+        <v>1699933</v>
       </c>
       <c r="F187">
-        <v>94702</v>
+        <v>100442</v>
       </c>
       <c r="G187">
-        <v>289.4603501398614</v>
+        <v>307.0048836217605</v>
       </c>
       <c r="H187">
-        <v>4821.039125795142</v>
+        <v>5195.911399910297</v>
       </c>
       <c r="I187">
-        <v>6.004107052172496</v>
+        <v>5.908585808970118</v>
       </c>
     </row>
     <row r="188">
@@ -6925,19 +6925,19 @@
         <v>32955400</v>
       </c>
       <c r="E188">
-        <v>3006</v>
+        <v>3333</v>
       </c>
       <c r="F188">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G188">
-        <v>0.3944725295399237</v>
+        <v>0.4248165702737639</v>
       </c>
       <c r="H188">
-        <v>91.21418644592389</v>
+        <v>101.1366877658896</v>
       </c>
       <c r="I188">
-        <v>0.4324683965402528</v>
+        <v>0.42004200420042</v>
       </c>
     </row>
     <row r="189">
@@ -7030,19 +7030,19 @@
         <v>28870195</v>
       </c>
       <c r="E191">
-        <v>882</v>
+        <v>1245</v>
       </c>
       <c r="F191">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G191">
-        <v>0.3463779860163743</v>
+        <v>0.3810157846180118</v>
       </c>
       <c r="H191">
-        <v>30.55053836664422</v>
+        <v>43.1240592590386</v>
       </c>
       <c r="I191">
-        <v>1.133786848072562</v>
+        <v>0.8835341365461846</v>
       </c>
     </row>
     <row r="192">
@@ -7100,7 +7100,7 @@
         <v>95540395</v>
       </c>
       <c r="E193">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="F193">
         <v>0</v>
@@ -7109,7 +7109,7 @@
         <v>0</v>
       </c>
       <c r="H193">
-        <v>3.39123571762499</v>
+        <v>3.42263604834374</v>
       </c>
       <c r="I193">
         <v>0</v>
@@ -7135,19 +7135,19 @@
         <v>28498687</v>
       </c>
       <c r="E194">
-        <v>193</v>
+        <v>255</v>
       </c>
       <c r="F194">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="G194">
-        <v>1.157948083713471</v>
+        <v>1.859734801115574</v>
       </c>
       <c r="H194">
-        <v>6.772241822930298</v>
+        <v>8.947780646876819</v>
       </c>
       <c r="I194">
-        <v>17.09844559585492</v>
+        <v>20.7843137254902</v>
       </c>
     </row>
     <row r="195">
@@ -7170,19 +7170,19 @@
         <v>57779622</v>
       </c>
       <c r="E195">
-        <v>19137</v>
+        <v>25937</v>
       </c>
       <c r="F195">
-        <v>369</v>
+        <v>552</v>
       </c>
       <c r="G195">
-        <v>6.386334614650127</v>
+        <v>9.553541212159539</v>
       </c>
       <c r="H195">
-        <v>331.2067358280745</v>
+        <v>448.8952869923586</v>
       </c>
       <c r="I195">
-        <v>1.928201912525474</v>
+        <v>2.12823379727802</v>
       </c>
     </row>
     <row r="196">
@@ -7205,7 +7205,7 @@
         <v>17351822</v>
       </c>
       <c r="E196">
-        <v>866</v>
+        <v>1057</v>
       </c>
       <c r="F196">
         <v>7</v>
@@ -7214,10 +7214,10 @@
         <v>0.4034158487794538</v>
       </c>
       <c r="H196">
-        <v>49.90830357757243</v>
+        <v>60.91579316569752</v>
       </c>
       <c r="I196">
-        <v>0.8083140877598153</v>
+        <v>0.6622516556291391</v>
       </c>
     </row>
     <row r="197">
@@ -7240,7 +7240,7 @@
         <v>14439018</v>
       </c>
       <c r="E197">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="F197">
         <v>4</v>
@@ -7249,10 +7249,10 @@
         <v>0.2770271496302588</v>
       </c>
       <c r="H197">
-        <v>3.5320961577858</v>
+        <v>9.141895937798541</v>
       </c>
       <c r="I197">
-        <v>7.84313725490196</v>
+        <v>3.03030303030303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>